<commit_message>
balance the card attr of level, star and quality
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/BattleMap.xlsx
+++ b/ConfigData/Xlsx/BattleMap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1257,7 +1257,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1291,7 +1291,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fix a bug of null magic def useless.
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/BattleMap.xlsx
+++ b/ConfigData/Xlsx/BattleMap.xlsx
@@ -90,32 +90,28 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>0;4;51018002;2;1;51018003;2;7;51018003</t>
-  </si>
-  <si>
-    <t>19;4;51018002;17;1;51018003;17;7;51018003</t>
-  </si>
-  <si>
-    <t>0;2;51018002</t>
-  </si>
-  <si>
-    <t>10;2;51018002</t>
-  </si>
-  <si>
-    <t>8;4;51018002</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;2;51018002</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>9;2;51018002</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>14;4;51018002</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>1;2;51018001</t>
+  </si>
+  <si>
+    <t>9;2;51018001</t>
+  </si>
+  <si>
+    <t>0;2;51018001</t>
+  </si>
+  <si>
+    <t>10;2;51018001</t>
+  </si>
+  <si>
+    <t>8;4;51018001</t>
+  </si>
+  <si>
+    <t>14;4;51018001</t>
+  </si>
+  <si>
+    <t>0;4;51018001;2;1;51018002;2;7;51018002</t>
+  </si>
+  <si>
+    <t>19;4;51018001;17;1;51018002;17;7;51018002</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1167,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1251,10 +1247,10 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F4" s="5">
         <v>3</v>
@@ -1268,10 +1264,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F5" s="5">
         <v>2</v>
@@ -1305,7 +1301,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
uniform the load battlefile mechanical
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/BattleMap.xlsx
+++ b/ConfigData/Xlsx/BattleMap.xlsx
@@ -90,30 +90,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;2;51018001</t>
-  </si>
-  <si>
-    <t>9;2;51018001</t>
-  </si>
-  <si>
-    <t>0;2;51018001</t>
-  </si>
-  <si>
-    <t>10;2;51018001</t>
-  </si>
-  <si>
-    <t>8;4;51018001</t>
-  </si>
-  <si>
-    <t>14;4;51018001</t>
-  </si>
-  <si>
-    <t>0;4;51018001;2;1;51018002;2;7;51018002</t>
-  </si>
-  <si>
-    <t>19;4;51018001;17;1;51018002;17;7;51018002</t>
-  </si>
-  <si>
     <t>均衡列</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -147,6 +123,38 @@
   </si>
   <si>
     <t>8;9;10;11</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>510180010;4;;51018002;2;1;51018002;2;7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018001;19;4;51018002;17;1;51018002;17;7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018001;1;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018001;0;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018001;10;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018001;9;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018001;8;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>51018001;14;4</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1279,7 +1287,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1287,8 +1295,8 @@
     <col min="1" max="1" width="8.875" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="27.75" customWidth="1"/>
-    <col min="5" max="5" width="28.125" customWidth="1"/>
+    <col min="4" max="4" width="49.25" customWidth="1"/>
+    <col min="5" max="5" width="58" customWidth="1"/>
     <col min="6" max="6" width="5.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1312,10 +1320,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -1364,10 +1372,10 @@
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
@@ -1378,19 +1386,19 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5">
         <v>3</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -1401,10 +1409,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F5" s="5">
         <v>2</v>
@@ -1413,7 +1421,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -1424,10 +1432,10 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F6" s="5">
         <v>3</v>
@@ -1436,7 +1444,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
@@ -1447,19 +1455,19 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F7" s="5">
         <v>2</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>